<commit_message>
added function to update from direct keyword match
</commit_message>
<xml_diff>
--- a/data/exceptions.xlsx
+++ b/data/exceptions.xlsx
@@ -295,12 +295,12 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,11 +832,6 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
exception tag update module implemented and tested
</commit_message>
<xml_diff>
--- a/data/exceptions.xlsx
+++ b/data/exceptions.xlsx
@@ -292,15 +292,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,6 +832,8 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
ML model imported, implementation successful
</commit_message>
<xml_diff>
--- a/data/exceptions.xlsx
+++ b/data/exceptions.xlsx
@@ -294,13 +294,13 @@
   </sheetPr>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="58.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="80.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>